<commit_message>
VAT code until final consumption
- R code updated
- Canada inputs updated
- US still missing
- Final consumption figures missing in the OECD data explorer.
</commit_message>
<xml_diff>
--- a/source_data/Canada_VAT.xlsx
+++ b/source_data/Canada_VAT.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBCB94A8-BDD4-4750-9F73-54B3610E09AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1638C2B3-B0BC-400E-A964-3C45A47D7699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{DC2465AE-7D70-4E8A-BA73-074BB36453DC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{DC2465AE-7D70-4E8A-BA73-074BB36453DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2023" sheetId="1" r:id="rId1"/>
+    <sheet name="2024" sheetId="2" r:id="rId2"/>
+    <sheet name="2025" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="26">
   <si>
     <t>Province</t>
   </si>
@@ -108,6 +110,12 @@
   </si>
   <si>
     <t>Weighted average</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>As of April 1, 2025, the HST was reduced from 15% to 14%.</t>
   </si>
 </sst>
 </file>
@@ -115,7 +123,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -154,12 +162,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,9 +189,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -219,7 +229,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -325,7 +335,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -467,7 +477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12E7EFA2-BABA-4C87-8650-036731404038}">
-  <dimension ref="A2:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -487,44 +497,62 @@
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4601314</v>
+      </c>
+      <c r="E2" s="4">
+        <f>D2/$D$15</f>
+        <v>0.11710456143440626</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="D3" s="3">
-        <v>4601314</v>
+        <v>5368266</v>
       </c>
       <c r="E3" s="4">
-        <f>D3/$D$16</f>
-        <v>0.11710456143440626</v>
+        <f t="shared" ref="E3:E15" si="0">D3/$D$15</f>
+        <v>0.13662367653962201</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -533,34 +561,34 @@
         <v>0.12</v>
       </c>
       <c r="D4" s="3">
-        <v>5368266</v>
+        <v>1420228</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E16" si="0">D4/$D$16</f>
-        <v>0.13662367653962201</v>
+        <f t="shared" si="0"/>
+        <v>3.6145148337380133E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="D5" s="3">
-        <v>1420228</v>
+        <v>820786</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>3.6145148337380133E-2</v>
+        <v>2.0889203510453879E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -569,202 +597,884 @@
         <v>0.15</v>
       </c>
       <c r="D6" s="3">
-        <v>820786</v>
+        <v>528818</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2.0889203510453879E-2</v>
+        <v>1.3458546834365107E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="D7" s="3">
-        <v>528818</v>
+        <v>45602</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1.3458546834365107E-2</v>
+        <v>1.1605820012569874E-3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="1">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="D8" s="3">
-        <v>45602</v>
+        <v>1030953</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>1.1605820012569874E-3</v>
+        <v>2.6238004823075634E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="D9" s="3">
-        <v>1030953</v>
+        <v>40586</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2.6238004823075634E-2</v>
+        <v>1.0329235801722753E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1">
-        <v>0.05</v>
+        <v>0.13</v>
       </c>
       <c r="D10" s="3">
-        <v>40586</v>
+        <v>15262660</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>1.0329235801722753E-3</v>
+        <v>0.38843841251052524</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="D11" s="3">
-        <v>15262660</v>
+        <v>172707</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>0.38843841251052524</v>
+        <v>4.3954351934364843E-3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.15</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.14974999999999999</v>
       </c>
       <c r="D12" s="3">
-        <v>172707</v>
+        <v>8751352</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>4.3954351934364843E-3</v>
+        <v>0.22272403881111225</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.14974999999999999</v>
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.11</v>
       </c>
       <c r="D13" s="3">
-        <v>8751352</v>
+        <v>1205119</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>0.22272403881111225</v>
+        <v>3.0670571921688074E-2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>0.11</v>
+        <v>0.05</v>
       </c>
       <c r="D14" s="3">
-        <v>1205119</v>
+        <v>43964</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3.0670571921688074E-2</v>
+        <v>1.11889450250564E-3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.05</v>
+        <v>22</v>
+      </c>
+      <c r="C15" s="4">
+        <f>AVERAGE(C2:C14)</f>
+        <v>0.10998076923076926</v>
       </c>
       <c r="D15" s="3">
-        <v>43964</v>
+        <f>SUM(D2:D14)</f>
+        <v>39292355</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>1.11889450250564E-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4">
-        <f>AVERAGE(C3:C15)</f>
-        <v>0.10998076923076926</v>
-      </c>
-      <c r="D16" s="3">
-        <f>SUM(D3:D15)</f>
-        <v>39292355</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="4">
-        <f>SUMPRODUCT(C3:C15,E3:E15)</f>
+        <f>SUMPRODUCT(C2:C14,E2:E14)</f>
         <v>0.12372396696507501</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCEA0AD-9F1C-4971-9421-DC0E5B40F306}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="10.1328125" customWidth="1"/>
+    <col min="7" max="9" width="9.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="5">
+        <v>4791876</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2/$D$15</f>
+        <v>0.11749299167553363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="D3" s="5">
+        <v>5627961</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E14" si="0">D3/$D$15</f>
+        <v>0.13799313148404255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1475046</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>3.6166955780790065E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D5" s="5">
+        <v>844433</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.0704826134805218E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="5">
+        <v>541820</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>1.328499584497546E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="5">
+        <v>44499</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.091080119053492E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1068120</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.6189453622854804E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D9" s="5">
+        <v>40794</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0002364632164353E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="D10" s="5">
+        <v>15944379</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.39094350294509983</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="5">
+        <v>176318</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3231772496297354E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.14974999999999999</v>
+      </c>
+      <c r="D12" s="5">
+        <v>8956326</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.21960199641254602</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1226848</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0081338050305367E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45936</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1263142171473789E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4">
+        <f>AVERAGE(C2:C14)</f>
+        <v>0.10998076923076926</v>
+      </c>
+      <c r="D15" s="3">
+        <v>40784356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4">
+        <f>SUMPRODUCT(C2:C14,E2:E14)</f>
+        <v>0.12362711105454258</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+      <c r="H37" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E9E7BA-0FF7-4168-B8FA-128BBF20D3FB}">
+  <dimension ref="A1:I34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="10.1328125" customWidth="1"/>
+    <col min="8" max="9" width="9.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D2" s="5">
+        <v>4960097</v>
+      </c>
+      <c r="E2" s="6">
+        <f>D2/$D$15</f>
+        <v>0.11943786799869391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="D3" s="5">
+        <v>5722318</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E14" si="0">D3/$D$15</f>
+        <v>0.13779195486107432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1504023</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>3.621648942369466E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D5" s="5">
+        <v>858963</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>2.0683609495895365E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="5">
+        <v>545579</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3137402874350931E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45074</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0853703994444322E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1079627</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5997142215933664E-2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D9" s="5">
+        <v>41414</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>9.9723853491129506E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="D10" s="5">
+        <v>16182641</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.38967385912578967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="D11" s="5">
+        <v>179280</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3170165774592401E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.14974999999999999</v>
+      </c>
+      <c r="D12" s="5">
+        <v>9111629</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.21940569746016489</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1250909</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0121568997618031E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D14" s="5">
+        <v>47126</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>1.134782034969568E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4">
+        <f>AVERAGE(C2:C14)</f>
+        <v>0.10921153846153848</v>
+      </c>
+      <c r="D15" s="3">
+        <v>41528680</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="4">
+        <f>SUMPRODUCT(C2:C14,E2:E14)</f>
+        <v>0.12320105798571011</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I34" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>